<commit_message>
fix bug # 118414 #118168
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR005.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KWR005.xlsx
@@ -240,47 +240,47 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -623,7 +623,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -637,7 +637,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="9.28515625" style="19"/>
+    <col min="1" max="2" width="9.28515625" style="13"/>
     <col min="3" max="1025" width="9.28515625" style="4"/>
     <col min="1026" max="16384" width="9.28515625" style="5"/>
   </cols>
@@ -676,55 +676,55 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="12" customHeight="1" thickBot="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="10"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="8"/>
     </row>
     <row r="4" spans="1:15" ht="12" customHeight="1">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="14"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="12" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -733,7 +733,7 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.78740157480314965" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>